<commit_message>
Large Transportation problem done
</commit_message>
<xml_diff>
--- a/docs/io.xlsx
+++ b/docs/io.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Capacities" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="40">
   <si>
     <t xml:space="preserve">NodeIndex</t>
   </si>
@@ -239,7 +239,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,6 +250,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -322,7 +328,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -423,6 +429,14 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,6 +446,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -442,11 +516,11 @@
   </sheetPr>
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.01"/>
@@ -1502,13 +1576,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E166"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E171" activeCellId="0" sqref="E171"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="17" width="11.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="19.72"/>
@@ -4003,6 +4077,90 @@
         <v>1</v>
       </c>
       <c r="E166" s="20"/>
+    </row>
+    <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B167" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C167" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" s="26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B168" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C168" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D168" s="26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C169" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" s="26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B170" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C170" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D170" s="26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C171" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D171" s="26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B172" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C172" s="25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D172" s="26" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>